<commit_message>
Fix some mistyped values in the benchmark xls
</commit_message>
<xml_diff>
--- a/docs/benchmark/benchmark.xlsx
+++ b/docs/benchmark/benchmark.xlsx
@@ -244,7 +244,7 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>4.37E-4</c:v>
+                  <c:v>1.07E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.02E-4</c:v>
@@ -262,11 +262,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="74289536"/>
-        <c:axId val="74291840"/>
+        <c:axId val="75665792"/>
+        <c:axId val="75668096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="74289536"/>
+        <c:axId val="75665792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -291,14 +291,14 @@
         </c:title>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74291840"/>
+        <c:crossAx val="75668096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74291840"/>
+        <c:axId val="75668096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -324,7 +324,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74289536"/>
+        <c:crossAx val="75665792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -502,11 +502,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="74308992"/>
-        <c:axId val="84620800"/>
+        <c:axId val="75685248"/>
+        <c:axId val="85603840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="74308992"/>
+        <c:axId val="75685248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -532,14 +532,14 @@
         <c:numFmt formatCode="@" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84620800"/>
+        <c:crossAx val="85603840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84620800"/>
+        <c:axId val="85603840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -565,7 +565,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74308992"/>
+        <c:crossAx val="75685248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -593,16 +593,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>136072</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -623,16 +623,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>704369</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>168089</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>704369</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>120063</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1220,8 +1220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="E17" zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1399,7 +1399,7 @@
         <v>1</v>
       </c>
       <c r="B14">
-        <v>4.37E-4</v>
+        <v>1.07E-4</v>
       </c>
       <c r="C14" s="2">
         <v>1.02E-4</v>

</xml_diff>